<commit_message>
include more origin countries, update of description
</commit_message>
<xml_diff>
--- a/country_characteristics_description and source.xlsx
+++ b/country_characteristics_description and source.xlsx
@@ -12,14 +12,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="variables" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="122">
   <si>
     <t>year</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Destination ISO3 alphabetic</t>
   </si>
   <si>
-    <t>1 = Contiguity</t>
-  </si>
-  <si>
     <t>Distance between most populated cities, in km</t>
   </si>
   <si>
@@ -198,12 +195,6 @@
     <t>Trade flow, 1000 USD (source: BACI)</t>
   </si>
   <si>
-    <t>Dummy variable if origin has been independent at a given year</t>
-  </si>
-  <si>
-    <t>Dummy variable if destination has been independent at a given year</t>
-  </si>
-  <si>
     <t>Bilateral de-facto exchange rate regime</t>
   </si>
   <si>
@@ -219,36 +210,6 @@
     <t>Currency destination</t>
   </si>
   <si>
-    <t>Voice and Accountability, Estimate</t>
-  </si>
-  <si>
-    <t>Political Stability and Absence of Violence/Terrorism, Estimate</t>
-  </si>
-  <si>
-    <t>Government Effectiveness, Estimate</t>
-  </si>
-  <si>
-    <t>Regulatory Quality, Estimate</t>
-  </si>
-  <si>
-    <t>Rule of Law, Estimate</t>
-  </si>
-  <si>
-    <t>Control of Corruption, Estimate</t>
-  </si>
-  <si>
-    <t>Export invoice percentage shares in USD</t>
-  </si>
-  <si>
-    <t>Export invoice percentage shares in EUR (including legacy currencies)</t>
-  </si>
-  <si>
-    <t>Import invoice percentage shares in USD</t>
-  </si>
-  <si>
-    <t>Import invoice percentage shares in EUR (including legacy currencies)</t>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
@@ -303,9 +264,6 @@
     <t xml:space="preserve"> http://www.cepii.fr/CEPII/en/bdd_modele/presentation.asp?id=20</t>
   </si>
   <si>
-    <t>Harms&amp;Knaze 2018</t>
-  </si>
-  <si>
     <t>https://www.international.economics.uni-mainz.de/data-on-bilateral-exchange-rate-regimes/</t>
   </si>
   <si>
@@ -358,13 +316,146 @@
   </si>
   <si>
     <t>https://www.imf.org/en/Publications/WP/Issues/2020/07/17/Patterns-in-Invoicing-Currency-in-Global-Trade-49581</t>
+  </si>
+  <si>
+    <t>1 = Contiguity (common border)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Origin country: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Voice and Accountability, Estimate</t>
+    </r>
+  </si>
+  <si>
+    <t>Origin country: Political Stability and Absence of Violence/Terrorism, Estimate</t>
+  </si>
+  <si>
+    <t>Origin country: Government Effectiveness, Estimate</t>
+  </si>
+  <si>
+    <t>Origin country: Regulatory Quality, Estimate</t>
+  </si>
+  <si>
+    <t>Origin country: Rule of Law, Estimate</t>
+  </si>
+  <si>
+    <t>Origin country: Control of Corruption, Estimate</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Destination country: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Voice and Accountability, Estimate</t>
+    </r>
+  </si>
+  <si>
+    <t>Destination country: Political Stability and Absence of Violence/Terrorism, Estimate</t>
+  </si>
+  <si>
+    <t>Destination country: Government Effectiveness, Estimate</t>
+  </si>
+  <si>
+    <t>Destination country: Regulatory Quality, Estimate</t>
+  </si>
+  <si>
+    <t>Destination country: Rule of Law, Estimate</t>
+  </si>
+  <si>
+    <t>Destination country: Control of Corruption, Estimate</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Origin country:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Export invoice percentage shares in USD</t>
+    </r>
+  </si>
+  <si>
+    <t>Origin country: Export invoice percentage shares in EUR</t>
+  </si>
+  <si>
+    <t>Origin country: Import invoice percentage shares in USD</t>
+  </si>
+  <si>
+    <t>Origin country: Import invoice percentage shares in EUR</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Destination country: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Export invoice percentage shares in USD</t>
+    </r>
+  </si>
+  <si>
+    <t>Destination country: Export invoice percentage shares in EUR</t>
+  </si>
+  <si>
+    <t>Destination country: Import invoice percentage shares in USD</t>
+  </si>
+  <si>
+    <t>Destination country: Import invoice percentage shares in EUR</t>
+  </si>
+  <si>
+    <t>Dummy = 1 if country is a sovereign, independent state (including cases of disputed sovereignty), otherwise 0</t>
+  </si>
+  <si>
+    <t>Harms&amp;Knaze 2018 based on Ilzetzki, Reinhardt, Rogoff (2018)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -384,6 +475,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -430,7 +527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -442,6 +539,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -723,36 +826,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.54296875" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -763,7 +866,7 @@
         <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -774,7 +877,7 @@
         <v>44</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -785,21 +888,21 @@
         <v>45</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>46</v>
+      <c r="B5" s="10" t="s">
+        <v>99</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -807,13 +910,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -821,13 +924,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -835,13 +938,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -849,13 +952,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -863,13 +966,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -877,13 +980,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -891,13 +994,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -905,13 +1008,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -919,13 +1022,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -933,13 +1036,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -947,426 +1050,428 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:6" ht="43.5">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>94</v>
+      <c r="B18" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>121</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>89</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="43.5">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>94</v>
+      <c r="B19" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>121</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>89</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="43.5">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>94</v>
+      <c r="B20" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="43.5">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>94</v>
+        <v>59</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.5">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>94</v>
+        <v>60</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>66</v>
+      <c r="B25" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>67</v>
+      <c r="B26" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>68</v>
+      <c r="B27" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>69</v>
+      <c r="B28" s="9" t="s">
+        <v>103</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>70</v>
+      <c r="B29" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>71</v>
+      <c r="B30" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
-        <v>66</v>
+      <c r="B31" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
-        <v>67</v>
+      <c r="B32" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
-        <v>68</v>
+      <c r="B33" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>69</v>
+      <c r="B34" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
-        <v>70</v>
+      <c r="B35" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
-        <v>71</v>
+      <c r="B36" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
-        <v>72</v>
+      <c r="B37" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="B38" t="s">
-        <v>73</v>
+      <c r="B38" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
-        <v>74</v>
+      <c r="B39" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
-        <v>75</v>
+      <c r="B40" s="9" t="s">
+        <v>115</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
-        <v>72</v>
+      <c r="B41" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>40</v>
       </c>
-      <c r="B42" t="s">
-        <v>73</v>
+      <c r="B42" s="9" t="s">
+        <v>117</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
-        <v>74</v>
+      <c r="B43" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>42</v>
       </c>
-      <c r="B44" t="s">
-        <v>75</v>
+      <c r="B44" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>